<commit_message>
Started translating the code_explanations
</commit_message>
<xml_diff>
--- a/code_explanations.xlsx
+++ b/code_explanations.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="100" windowWidth="31460" windowHeight="17820"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="21060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Türkçe" sheetId="1" r:id="rId1"/>
     <sheet name="English" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="204">
   <si>
     <t>Kod</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Trill</t>
   </si>
   <si>
-    <t>Nota dörde bölünür ve bunlar sessiz çarpmalı gibi seslendirilir. Daha çok sayıda tril yapılmak istenirse bu Pay ve Payda değerinde yazılmalıdır. Örneğin 1/4`lük bir nota normalde 1/16`lik dört sessiz çarpmalı notaya bölünür. Fakat Pay/Payda alanlarına 8/3</t>
-  </si>
-  <si>
     <t>Bekar Trill (-)</t>
   </si>
   <si>
@@ -550,13 +547,114 @@
   </si>
   <si>
     <t>Soz1=THM (indisli), Soz1=TSM (Arel – Ezgi. Bu takdirde b2’ler b1’e, b3’ler b4’e vb., yani sırasıyla ters ve çengelli bemole vb. dönüştürülmeli), Soz1=Karma (Mus2-Alfadaki yöntem)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Code2</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>Rest Symbol. Pay (numerator), Payda (denumerator) and LNS=100 is used</t>
+  </si>
+  <si>
+    <t>Generally used to show embellishments which are not originally on the piece but added in the performance. They are typically played softer than the other notes.</t>
+  </si>
+  <si>
+    <t>Rest (-)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acts as a normal note, however a rest with the same duration is given in the first occurence of this note. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acts as a normal note, however a rest with the same duration is given in the second occurence of this note. </t>
+  </si>
+  <si>
+    <t>Rest on the first occurence (-)</t>
+  </si>
+  <si>
+    <t>Rest on the second occurence (-)</t>
+  </si>
+  <si>
+    <t>Produces all pitches between the pitch of this note and the next note.</t>
+  </si>
+  <si>
+    <t>Attenuating Tremolo (-)</t>
+  </si>
+  <si>
+    <t>Amplifying Tremolo (-)</t>
+  </si>
+  <si>
+    <t>Note is performed as an tremolo getting softer by time.</t>
+  </si>
+  <si>
+    <t>Note is performed as an tremolo getting louder by time.</t>
+  </si>
+  <si>
+    <t>Note is not performed as a single onset but rather many onset. The total duration of all the onset would be equal to the duration of the note. In pieces where the tempo is less than 90 bpm taking a fourth notes the pulse unit, a tremolo typically correspond to 8 32nd notes. For faster pieces it will correspond to 4 16th notes.</t>
+  </si>
+  <si>
+    <t>A short and soft note which takes a its duration from the next note. For pieces slower than 4th note = 90bpm, it is a 64th note. For faster pieces it is a 32nd note. This duration is subtracted from the duration of the next note.</t>
+  </si>
+  <si>
+    <t>Normal note or rest if silence.
+Repeat signs:
+If there is "+" and "X" in the Söz-2 (Second lyrics column) field:
+   If LNS is 1, Dal Segno (D.S.), 
+   If LNS is 4, to the [Start] (to below),
+   If LNS is 5, to the (Start) (above the portrait); 
+If there is "]" or "}" in the Söz-2 field: 
+   LNS = 0 ise [SON], 
+   LNS = 1 ise [KA</t>
+  </si>
+  <si>
+    <t>Normal note. Gives some of its duration to the following grace note.</t>
+  </si>
+  <si>
+    <t>Note/Rest</t>
+  </si>
+  <si>
+    <t>Little Note</t>
+  </si>
+  <si>
+    <t>Gracenote</t>
+  </si>
+  <si>
+    <t>Note Followed by a Gracenote</t>
+  </si>
+  <si>
+    <t>Silent Gracenote</t>
+  </si>
+  <si>
+    <t>Normal note. Gives some of its duration to the following grace note with a pitch one degree sharper. This grace note is not shown and performed very softly.</t>
+  </si>
+  <si>
+    <t>The note is divided into four and played like silent gracenotes. If multiple trills are desired, it should be written to the Pay and Payda values. For example a 4th note is generally divided into four 16th notes; however if the Pay and Payda are 8 and 3, respectively XX</t>
+  </si>
+  <si>
+    <t>Nota dörde bölünür ve bunlar sessiz çarpmalı gibi seslendirilir. Daha çok sayıda tril yapılmak istenirse bu Pay ve Payda değerinde yazılmalıdır. Örneğin 1/4`lük bir nota normalde 1/16`lik dört sessiz çarpmalı notaya bölünür. Fakat Pay/Payda alanlarına 8/3 XX</t>
+  </si>
+  <si>
+    <t>Natural Trill (-)</t>
+  </si>
+  <si>
+    <t>If the note with the higher pitch in the scale has a flat or sharp, they are played as a natural.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -580,6 +678,22 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -636,9 +750,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -661,7 +777,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sayfa1" xfId="1"/>
   </cellStyles>
@@ -964,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1236,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>41</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="24">
@@ -1247,14 +1365,14 @@
         <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="60">
@@ -1262,17 +1380,17 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="36">
@@ -1283,14 +1401,14 @@
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="36">
@@ -1301,14 +1419,14 @@
         <v>8</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="24">
@@ -1319,7 +1437,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" s="3">
         <v>129</v>
@@ -1328,7 +1446,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="24">
@@ -1339,14 +1457,14 @@
         <v>8</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="6" t="b">
         <v>1</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1354,17 +1472,17 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="6" t="b">
         <v>1</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1375,14 +1493,14 @@
         <v>8</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="6" t="b">
         <v>1</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="24">
@@ -1390,17 +1508,17 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="6" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="24">
@@ -1411,14 +1529,14 @@
         <v>8</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="60">
@@ -1426,10 +1544,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="D25" s="3">
         <v>116</v>
@@ -1438,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="60">
@@ -1446,10 +1564,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="D26" s="3">
         <v>115</v>
@@ -1458,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1469,7 +1587,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="6" t="b">
@@ -1487,7 +1605,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="6" t="b">
@@ -1502,10 +1620,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="6" t="b">
@@ -1520,10 +1638,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="D30" s="3">
         <v>170</v>
@@ -1532,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60">
@@ -1540,10 +1658,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="D31" s="3">
         <v>168</v>
@@ -1552,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1563,7 +1681,7 @@
         <v>8</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="6" t="b">
@@ -1581,7 +1699,7 @@
         <v>8</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="6" t="b">
@@ -1596,10 +1714,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="D34" s="3">
         <v>165</v>
@@ -1608,7 +1726,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1619,7 +1737,7 @@
         <v>8</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="6" t="b">
@@ -1637,7 +1755,7 @@
         <v>8</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="6" t="b">
@@ -1652,10 +1770,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="D37" s="3">
         <v>212</v>
@@ -1664,7 +1782,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1675,14 +1793,14 @@
         <v>8</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="24">
@@ -1693,14 +1811,14 @@
         <v>8</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1711,7 +1829,7 @@
         <v>8</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="6" t="b">
@@ -1729,7 +1847,7 @@
         <v>8</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="6" t="b">
@@ -1747,7 +1865,7 @@
         <v>8</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="6" t="b">
@@ -1765,7 +1883,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="6" t="b">
@@ -1783,7 +1901,7 @@
         <v>8</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="6" t="b">
@@ -1798,10 +1916,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="D45" s="3">
         <v>194</v>
@@ -1810,7 +1928,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="60">
@@ -1818,10 +1936,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="D46" s="3">
         <v>188</v>
@@ -1830,7 +1948,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1841,7 +1959,7 @@
         <v>8</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="6" t="b">
@@ -1859,7 +1977,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="6" t="b">
@@ -1877,7 +1995,7 @@
         <v>8</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="6" t="b">
@@ -1895,7 +2013,7 @@
         <v>8</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="6" t="b">
@@ -1913,7 +2031,7 @@
         <v>8</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="6" t="b">
@@ -1928,17 +2046,17 @@
         <v>50</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="60">
@@ -1946,17 +2064,17 @@
         <v>51</v>
       </c>
       <c r="B53" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="60">
@@ -1964,17 +2082,17 @@
         <v>52</v>
       </c>
       <c r="B54" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="36">
@@ -1982,17 +2100,17 @@
         <v>53</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="6" t="b">
         <v>1</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="24">
@@ -2000,19 +2118,19 @@
         <v>54</v>
       </c>
       <c r="B56" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="D56" s="3">
+        <v>0</v>
+      </c>
+      <c r="E56" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="D56" s="3">
-        <v>0</v>
-      </c>
-      <c r="E56" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2020,19 +2138,19 @@
         <v>55</v>
       </c>
       <c r="B57" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="D57" s="3">
+        <v>0</v>
+      </c>
+      <c r="E57" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="D57" s="3">
-        <v>0</v>
-      </c>
-      <c r="E57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="48">
@@ -2040,19 +2158,19 @@
         <v>56</v>
       </c>
       <c r="B58" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="D58" s="3">
+        <v>0</v>
+      </c>
+      <c r="E58" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D58" s="3">
-        <v>0</v>
-      </c>
-      <c r="E58" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2060,19 +2178,19 @@
         <v>57</v>
       </c>
       <c r="B59" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="D59" s="3">
+        <v>0</v>
+      </c>
+      <c r="E59" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="D59" s="3">
-        <v>0</v>
-      </c>
-      <c r="E59" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="24">
@@ -2080,19 +2198,19 @@
         <v>58</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="D60" s="3">
+        <v>0</v>
+      </c>
+      <c r="E60" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="D60" s="3">
-        <v>0</v>
-      </c>
-      <c r="E60" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="24">
@@ -2100,19 +2218,19 @@
         <v>59</v>
       </c>
       <c r="B61" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="D61" s="3">
+        <v>0</v>
+      </c>
+      <c r="E61" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="D61" s="3">
-        <v>0</v>
-      </c>
-      <c r="E61" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2120,19 +2238,19 @@
         <v>60</v>
       </c>
       <c r="B62" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="D62" s="3">
+        <v>0</v>
+      </c>
+      <c r="E62" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="D62" s="3">
-        <v>0</v>
-      </c>
-      <c r="E62" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="48">
@@ -2143,16 +2261,16 @@
         <v>8</v>
       </c>
       <c r="C63" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D63" s="3">
+        <v>0</v>
+      </c>
+      <c r="E63" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="D63" s="3">
-        <v>0</v>
-      </c>
-      <c r="E63" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2160,19 +2278,19 @@
         <v>62</v>
       </c>
       <c r="B64" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="D64" s="3">
+        <v>0</v>
+      </c>
+      <c r="E64" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="D64" s="3">
-        <v>0</v>
-      </c>
-      <c r="E64" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="48">
@@ -2180,11 +2298,11 @@
         <v>63</v>
       </c>
       <c r="B65" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>150</v>
-      </c>
       <c r="D65" s="3">
         <v>0</v>
       </c>
@@ -2192,7 +2310,7 @@
         <v>1</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="24">
@@ -2200,19 +2318,19 @@
         <v>64</v>
       </c>
       <c r="B66" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C66" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="D66" s="3">
+        <v>0</v>
+      </c>
+      <c r="E66" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="D66" s="3">
-        <v>0</v>
-      </c>
-      <c r="E66" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2220,19 +2338,19 @@
         <v>65</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="D67" s="3">
+        <v>0</v>
+      </c>
+      <c r="E67" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="D67" s="3">
-        <v>0</v>
-      </c>
-      <c r="E67" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2240,19 +2358,19 @@
         <v>66</v>
       </c>
       <c r="B68" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="D68" s="3">
+        <v>0</v>
+      </c>
+      <c r="E68" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="D68" s="3">
-        <v>0</v>
-      </c>
-      <c r="E68" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2260,19 +2378,19 @@
         <v>71</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="D69" s="3">
+        <v>0</v>
+      </c>
+      <c r="E69" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="D69" s="3">
-        <v>0</v>
-      </c>
-      <c r="E69" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2280,19 +2398,19 @@
         <v>72</v>
       </c>
       <c r="B70" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="D70" s="3">
+        <v>0</v>
+      </c>
+      <c r="E70" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="D70" s="3">
-        <v>0</v>
-      </c>
-      <c r="E70" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="24">
@@ -2300,19 +2418,19 @@
         <v>73</v>
       </c>
       <c r="B71" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="D71" s="3">
+        <v>0</v>
+      </c>
+      <c r="E71" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="D71" s="3">
-        <v>0</v>
-      </c>
-      <c r="E71" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="24">
@@ -2323,16 +2441,16 @@
         <v>8</v>
       </c>
       <c r="C72" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D72" s="3">
+        <v>0</v>
+      </c>
+      <c r="E72" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="D72" s="3">
-        <v>0</v>
-      </c>
-      <c r="E72" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="24">
@@ -2343,16 +2461,16 @@
         <v>8</v>
       </c>
       <c r="C73" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D73" s="3">
+        <v>0</v>
+      </c>
+      <c r="E73" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="4" t="s">
         <v>171</v>
-      </c>
-      <c r="D73" s="3">
-        <v>0</v>
-      </c>
-      <c r="E73" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2368,12 +2486,1400 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="24">
+      <c r="A1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="24">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="36">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="24">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="24">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="24">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="3">
+        <v>163</v>
+      </c>
+      <c r="E7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="72">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="48">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="3">
+        <v>227</v>
+      </c>
+      <c r="E10" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="120">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="24">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="36">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D13" s="3">
+        <v>218</v>
+      </c>
+      <c r="E13" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="60">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="3">
+        <v>164</v>
+      </c>
+      <c r="E14" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="24">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="60">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="36">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="36">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="24">
+      <c r="A19" s="3">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="3">
+        <v>129</v>
+      </c>
+      <c r="E19" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="24">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="24">
+      <c r="A23" s="3">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="24">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="60">
+      <c r="A25" s="3">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="3">
+        <v>116</v>
+      </c>
+      <c r="E25" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="60">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="3">
+        <v>115</v>
+      </c>
+      <c r="E26" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="3">
+        <v>25</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="24">
+      <c r="A29" s="3">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="60">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="3">
+        <v>170</v>
+      </c>
+      <c r="E30" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="60">
+      <c r="A31" s="3">
+        <v>29</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="3">
+        <v>168</v>
+      </c>
+      <c r="E31" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="3">
+        <v>31</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="60">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="3">
+        <v>165</v>
+      </c>
+      <c r="E34" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="3">
+        <v>33</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="3">
+        <v>34</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="24">
+      <c r="A37" s="3">
+        <v>35</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="3">
+        <v>212</v>
+      </c>
+      <c r="E37" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="3">
+        <v>36</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="24">
+      <c r="A39" s="3">
+        <v>37</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="3">
+        <v>38</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="3">
+        <v>39</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="3">
+        <v>40</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="3">
+        <v>41</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="3">
+        <v>42</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="60">
+      <c r="A45" s="3">
+        <v>43</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="3">
+        <v>194</v>
+      </c>
+      <c r="E45" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="60">
+      <c r="A46" s="3">
+        <v>44</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" s="3">
+        <v>188</v>
+      </c>
+      <c r="E46" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="3">
+        <v>45</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" s="5"/>
+      <c r="E47" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="3">
+        <v>46</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="3">
+        <v>47</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="24">
+      <c r="A50" s="3">
+        <v>48</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="E50" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="24">
+      <c r="A51" s="3">
+        <v>49</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="24">
+      <c r="A52" s="3">
+        <v>50</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D52" s="5"/>
+      <c r="E52" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="60">
+      <c r="A53" s="3">
+        <v>51</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="5"/>
+      <c r="E53" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="60">
+      <c r="A54" s="3">
+        <v>52</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="36">
+      <c r="A55" s="3">
+        <v>53</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" s="5"/>
+      <c r="E55" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="24">
+      <c r="A56" s="3">
+        <v>54</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0</v>
+      </c>
+      <c r="E56" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="3">
+        <v>55</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D57" s="3">
+        <v>0</v>
+      </c>
+      <c r="E57" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="48">
+      <c r="A58" s="3">
+        <v>56</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D58" s="3">
+        <v>0</v>
+      </c>
+      <c r="E58" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="3">
+        <v>57</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0</v>
+      </c>
+      <c r="E59" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="24">
+      <c r="A60" s="3">
+        <v>58</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D60" s="3">
+        <v>0</v>
+      </c>
+      <c r="E60" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="24">
+      <c r="A61" s="3">
+        <v>59</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D61" s="3">
+        <v>0</v>
+      </c>
+      <c r="E61" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="3">
+        <v>60</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D62" s="3">
+        <v>0</v>
+      </c>
+      <c r="E62" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="48">
+      <c r="A63" s="3">
+        <v>61</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D63" s="3">
+        <v>0</v>
+      </c>
+      <c r="E63" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="3">
+        <v>62</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D64" s="3">
+        <v>0</v>
+      </c>
+      <c r="E64" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="48">
+      <c r="A65" s="3">
+        <v>63</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D65" s="3">
+        <v>0</v>
+      </c>
+      <c r="E65" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="24">
+      <c r="A66" s="3">
+        <v>64</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D66" s="3">
+        <v>0</v>
+      </c>
+      <c r="E66" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="3">
+        <v>65</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D67" s="3">
+        <v>0</v>
+      </c>
+      <c r="E67" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="3">
+        <v>66</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D68" s="3">
+        <v>0</v>
+      </c>
+      <c r="E68" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="3">
+        <v>71</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D69" s="3">
+        <v>0</v>
+      </c>
+      <c r="E69" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="3">
+        <v>72</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D70" s="3">
+        <v>0</v>
+      </c>
+      <c r="E70" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="24">
+      <c r="A71" s="3">
+        <v>73</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D71" s="3">
+        <v>0</v>
+      </c>
+      <c r="E71" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="24">
+      <c r="A72" s="3">
+        <v>89</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D72" s="3">
+        <v>0</v>
+      </c>
+      <c r="E72" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="24">
+      <c r="A73" s="3">
+        <v>108</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D73" s="3">
+        <v>0</v>
+      </c>
+      <c r="E73" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Continuing cirrections in the makam/form/uusl dictionaries
</commit_message>
<xml_diff>
--- a/code_explanations.xlsx
+++ b/code_explanations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="235">
   <si>
     <t>Kod</t>
   </si>
@@ -600,9 +600,6 @@
     <t>Note is performed as an tremolo getting louder by time.</t>
   </si>
   <si>
-    <t>Note is not performed as a single onset but rather many onset. The total duration of all the onset would be equal to the duration of the note. In pieces where the tempo is less than 90 bpm taking a fourth notes the pulse unit, a tremolo typically correspond to 8 32nd notes. For faster pieces it will correspond to 4 16th notes.</t>
-  </si>
-  <si>
     <t>A short and soft note which takes a its duration from the next note. For pieces slower than 4th note = 90bpm, it is a 64th note. For faster pieces it is a 32nd note. This duration is subtracted from the duration of the next note.</t>
   </si>
   <si>
@@ -641,20 +638,116 @@
     <t>The note is divided into four and played like silent gracenotes. If multiple trills are desired, it should be written to the Pay and Payda values. For example a 4th note is generally divided into four 16th notes; however if the Pay and Payda are 8 and 3, respectively XX</t>
   </si>
   <si>
-    <t>Nota dörde bölünür ve bunlar sessiz çarpmalı gibi seslendirilir. Daha çok sayıda tril yapılmak istenirse bu Pay ve Payda değerinde yazılmalıdır. Örneğin 1/4`lük bir nota normalde 1/16`lik dört sessiz çarpmalı notaya bölünür. Fakat Pay/Payda alanlarına 8/3 XX</t>
-  </si>
-  <si>
     <t>Natural Trill (-)</t>
   </si>
   <si>
     <t>If the note with the higher pitch in the scale has a flat or sharp, they are played as a natural.</t>
+  </si>
+  <si>
+    <t>Nota dörde bölünür ve bunlar sessiz çarpmalı gibi seslendirilir. Daha çok sayıda tril yapılmak istenirse bu Pay ve Payda değerinde yazılmalıdır. Örneğin 1/4`lük bir nota normalde 1/16`lik dört sessiz çarpmalı notaya bölünür. Fakat Pay/Payda alanlarına 8/3 ??</t>
+  </si>
+  <si>
+    <t>Sonu silinmis</t>
+  </si>
+  <si>
+    <t>Missing the ending</t>
+  </si>
+  <si>
+    <t>Triole with Gracenote (-)</t>
+  </si>
+  <si>
+    <t>Triole with Soft Gracenote (-)</t>
+  </si>
+  <si>
+    <t>Makam/Change (-)</t>
+  </si>
+  <si>
+    <t>Usul/Change</t>
+  </si>
+  <si>
+    <t>Tempo/Change</t>
+  </si>
+  <si>
+    <t>Composer</t>
+  </si>
+  <si>
+    <t>Lyricist</t>
+  </si>
+  <si>
+    <t>Transposition (Ahenk)</t>
+  </si>
+  <si>
+    <t>Folkloric</t>
+  </si>
+  <si>
+    <t>Notation</t>
+  </si>
+  <si>
+    <t>Composition Date</t>
+  </si>
+  <si>
+    <t>Duration of the Composition</t>
+  </si>
+  <si>
+    <t>Paper Size</t>
+  </si>
+  <si>
+    <t>Margins</t>
+  </si>
+  <si>
+    <t>Vertical - Horizontal Layout</t>
+  </si>
+  <si>
+    <t>Written to the Söz1 field, e.g. "Şarkı, Peşrev"</t>
+  </si>
+  <si>
+    <t>Name - Surname of the composer (or explanation such as "Anonim" to indicate anonymous) is written to the Söz1 field. The birth and death dates are written to the Söz2 field.</t>
+  </si>
+  <si>
+    <t>Starting Lyrics</t>
+  </si>
+  <si>
+    <t>The first words of the lyrics, written to the Söz1 field</t>
+  </si>
+  <si>
+    <t>The transposition of the performance, given in Holderian commas. 9: Kızneyi nısfiyesi, 0: Mansur nısfiyesi (Default), -9: Şah nısfiyesi, -13: Davud nısfiyesi, -22: Bolahenk neyi, -31: Sipürde neyi, -35: Müstahzen neyi, -44: Kızneyi, -53: Mansur neyi</t>
+  </si>
+  <si>
+    <t>1 if the a folk music piece, 0 else</t>
+  </si>
+  <si>
+    <t>Soz1=THM (indiced accidentals; b1, b2 etc.), Soz1=TSM (Arel – Ezgi accidentals). Bu takdirde b2’ler b1’e, b3’ler b4’e vb., yani sırasıyla ters ve çengelli bemole vb. dönüştürülmeli), Soz1=Karma (Mus2-Alfadaki yöntem)</t>
+  </si>
+  <si>
+    <t>The date of composition written on the Söz1 field</t>
+  </si>
+  <si>
+    <t>The duration of the composition written in "x Dk y Sn" (Dk: minutes, Sn: seconds) to the Söz1 field</t>
+  </si>
+  <si>
+    <t>Pay field: Width, Payda field: Height (mm)</t>
+  </si>
+  <si>
+    <t>Pay field: Top, Payda field: Bottom; Bas field: Left, Çek field: Right (mm)</t>
+  </si>
+  <si>
+    <t>Pay field: The smallest interval, Payda field: Highest note in the line; Bas field: Line spacing, Çek: Punto</t>
+  </si>
+  <si>
+    <t>Note is not performed as a single onset but rather many onset. The total duration of all the onset would be equal to the duration of the note. In pieces where the tempo is less than 4th note = 90 bpm, a tremolo typically corresponds to eight 32nd notes. For faster pieces it corresponds to four 16th notes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used to indicate a tempo change. The value in the Legato% field indicates the tempo starting from this point now on. If the value is greater than 127, the sum of this value, and the values in the Basış and Bırakış fields indicate the tempo. In the Pay, Payda fields, XX </t>
+  </si>
+  <si>
+    <t>Sonu silinmiş</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -696,8 +789,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -708,6 +806,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
         <bgColor indexed="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -750,13 +854,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -776,10 +884,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sayfa1" xfId="1"/>
   </cellStyles>
@@ -1080,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A39" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1095,7 +1213,7 @@
     <col min="6" max="6" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1133,7 +1251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="36">
+    <row r="3" spans="1:7" ht="36">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1151,7 +1269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24">
+    <row r="4" spans="1:7" ht="24">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1169,7 +1287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24">
+    <row r="5" spans="1:7" ht="24">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1187,7 +1305,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24">
+    <row r="6" spans="1:7" ht="24">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1205,7 +1323,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1225,7 +1343,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1243,7 +1361,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="48">
+    <row r="9" spans="1:7" ht="48">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1261,7 +1379,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="48">
+    <row r="10" spans="1:7" ht="48">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1281,7 +1399,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="108">
+    <row r="11" spans="1:7" ht="108">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1299,7 +1417,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="24">
+    <row r="12" spans="1:7" ht="24">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1317,7 +1435,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="36">
+    <row r="13" spans="1:7" ht="36">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1337,7 +1455,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60">
+    <row r="14" spans="1:7" ht="60">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1353,11 +1471,14 @@
       <c r="E14" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="24">
+      <c r="F14" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="G14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="24">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1375,7 +1496,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="60">
+    <row r="16" spans="1:7" ht="60">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1987,7 +2108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:7">
       <c r="A49" s="3">
         <v>47</v>
       </c>
@@ -2005,7 +2126,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="24">
+    <row r="50" spans="1:7" ht="24">
       <c r="A50" s="3">
         <v>48</v>
       </c>
@@ -2023,7 +2144,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="24">
+    <row r="51" spans="1:7" ht="24">
       <c r="A51" s="3">
         <v>49</v>
       </c>
@@ -2041,7 +2162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="24">
+    <row r="52" spans="1:7" ht="24">
       <c r="A52" s="3">
         <v>50</v>
       </c>
@@ -2059,7 +2180,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="60">
+    <row r="53" spans="1:7" ht="60">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -2073,11 +2194,14 @@
       <c r="E53" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="F53" s="7" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="60">
+      <c r="G53" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="60">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -2091,11 +2215,14 @@
       <c r="E54" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F54" s="4" t="s">
+      <c r="F54" s="8" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="36">
+      <c r="G54" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="36">
       <c r="A55" s="3">
         <v>53</v>
       </c>
@@ -2113,7 +2240,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="24">
+    <row r="56" spans="1:7" ht="24">
       <c r="A56" s="3">
         <v>54</v>
       </c>
@@ -2133,7 +2260,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:7">
       <c r="A57" s="3">
         <v>55</v>
       </c>
@@ -2153,7 +2280,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="48">
+    <row r="58" spans="1:7" ht="48">
       <c r="A58" s="3">
         <v>56</v>
       </c>
@@ -2173,7 +2300,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:7">
       <c r="A59" s="3">
         <v>57</v>
       </c>
@@ -2193,7 +2320,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="24">
+    <row r="60" spans="1:7" ht="24">
       <c r="A60" s="3">
         <v>58</v>
       </c>
@@ -2213,7 +2340,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="24">
+    <row r="61" spans="1:7" ht="24">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -2233,7 +2360,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:7">
       <c r="A62" s="3">
         <v>60</v>
       </c>
@@ -2253,7 +2380,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="48">
+    <row r="63" spans="1:7" ht="48">
       <c r="A63" s="3">
         <v>61</v>
       </c>
@@ -2273,7 +2400,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:7">
       <c r="A64" s="3">
         <v>62</v>
       </c>
@@ -2486,10 +2613,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2501,7 +2628,7 @@
     <col min="6" max="6" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24">
+    <row r="1" spans="1:7" ht="24">
       <c r="A1" s="1" t="s">
         <v>174</v>
       </c>
@@ -2521,7 +2648,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="24">
+    <row r="2" spans="1:7" ht="24">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -2539,7 +2666,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="36">
+    <row r="3" spans="1:7" ht="36">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2547,7 +2674,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6" t="b">
@@ -2557,7 +2684,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24">
+    <row r="4" spans="1:7" ht="24">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2575,7 +2702,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24">
+    <row r="5" spans="1:7" ht="24">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2593,7 +2720,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24">
+    <row r="6" spans="1:7" ht="24">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2611,7 +2738,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2631,7 +2758,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -2649,7 +2776,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="72">
+    <row r="9" spans="1:7" ht="72">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2664,10 +2791,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="48">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="48">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2675,7 +2802,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D10" s="3">
         <v>227</v>
@@ -2684,10 +2811,10 @@
         <v>0</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="120">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="120">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2695,17 +2822,17 @@
         <v>30</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="24">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="24">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2713,17 +2840,17 @@
         <v>33</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="36">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="36">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2731,7 +2858,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" s="3">
         <v>218</v>
@@ -2740,10 +2867,10 @@
         <v>0</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="60">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="60">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2759,11 +2886,14 @@
       <c r="E14" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="24">
+      <c r="F14" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="G14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="24">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2771,31 +2901,31 @@
         <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="60">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="7" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2806,14 +2936,14 @@
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="7" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2824,14 +2954,14 @@
       <c r="B18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="7" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2842,7 +2972,7 @@
       <c r="B19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="7" t="s">
         <v>50</v>
       </c>
       <c r="D19" s="3">
@@ -2851,7 +2981,7 @@
       <c r="E19" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2862,14 +2992,14 @@
       <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="7" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2880,14 +3010,14 @@
       <c r="B21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="7" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2898,14 +3028,14 @@
       <c r="B22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="7" t="s">
         <v>57</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2916,14 +3046,14 @@
       <c r="B23" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="7" t="s">
         <v>60</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="7" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2934,14 +3064,14 @@
       <c r="B24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="7" t="s">
         <v>62</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="7" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2952,7 +3082,7 @@
       <c r="B25" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D25" s="3">
@@ -2961,7 +3091,7 @@
       <c r="E25" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2972,7 +3102,7 @@
       <c r="B26" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D26" s="3">
@@ -2981,7 +3111,7 @@
       <c r="E26" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="7" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2992,14 +3122,14 @@
       <c r="B27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="7" t="s">
         <v>70</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3010,14 +3140,14 @@
       <c r="B28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="7" t="s">
         <v>71</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3028,14 +3158,14 @@
       <c r="B29" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="7" t="s">
         <v>73</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3046,7 +3176,7 @@
       <c r="B30" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="7" t="s">
         <v>75</v>
       </c>
       <c r="D30" s="3">
@@ -3055,7 +3185,7 @@
       <c r="E30" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="7" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3066,7 +3196,7 @@
       <c r="B31" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D31" s="3">
@@ -3075,7 +3205,7 @@
       <c r="E31" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="7" t="s">
         <v>79</v>
       </c>
     </row>
@@ -3086,14 +3216,14 @@
       <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3104,14 +3234,14 @@
       <c r="B33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="7" t="s">
         <v>81</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F33" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3122,7 +3252,7 @@
       <c r="B34" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D34" s="3">
@@ -3131,7 +3261,7 @@
       <c r="E34" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="7" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3143,13 +3273,13 @@
         <v>8</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>85</v>
+        <v>205</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3161,13 +3291,13 @@
         <v>8</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>86</v>
+        <v>206</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3178,7 +3308,7 @@
       <c r="B37" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D37" s="3">
@@ -3187,7 +3317,7 @@
       <c r="E37" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="7" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3198,14 +3328,14 @@
       <c r="B38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="7" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3223,7 +3353,7 @@
       <c r="E39" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="7" t="s">
         <v>93</v>
       </c>
     </row>
@@ -3241,7 +3371,7 @@
       <c r="E40" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3259,7 +3389,7 @@
       <c r="E41" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3277,7 +3407,7 @@
       <c r="E42" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3295,7 +3425,7 @@
       <c r="E43" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F43" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3313,7 +3443,7 @@
       <c r="E44" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3324,7 +3454,7 @@
       <c r="B45" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="7" t="s">
         <v>100</v>
       </c>
       <c r="D45" s="3">
@@ -3333,7 +3463,7 @@
       <c r="E45" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F45" s="7" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3344,7 +3474,7 @@
       <c r="B46" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="7" t="s">
         <v>103</v>
       </c>
       <c r="D46" s="3">
@@ -3353,7 +3483,7 @@
       <c r="E46" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F46" s="7" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3364,7 +3494,7 @@
       <c r="B47" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="7" t="s">
         <v>105</v>
       </c>
       <c r="D47" s="5"/>
@@ -3382,7 +3512,7 @@
       <c r="B48" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D48" s="5"/>
@@ -3400,7 +3530,7 @@
       <c r="B49" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="7" t="s">
         <v>107</v>
       </c>
       <c r="D49" s="5"/>
@@ -3418,7 +3548,7 @@
       <c r="B50" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="7" t="s">
         <v>108</v>
       </c>
       <c r="D50" s="5"/>
@@ -3436,7 +3566,7 @@
       <c r="B51" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="7" t="s">
         <v>109</v>
       </c>
       <c r="D51" s="5"/>
@@ -3455,13 +3585,13 @@
         <v>110</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>111</v>
+        <v>207</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="F52" s="7" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3473,13 +3603,13 @@
         <v>113</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>114</v>
+        <v>208</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="F53" s="7" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3491,14 +3621,14 @@
         <v>116</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>117</v>
+        <v>209</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F54" s="4" t="s">
-        <v>118</v>
+      <c r="F54" s="7" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="36">
@@ -3508,14 +3638,14 @@
       <c r="B55" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="7" t="s">
         <v>120</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F55" s="7" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3526,7 +3656,7 @@
       <c r="B56" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="7" t="s">
         <v>123</v>
       </c>
       <c r="D56" s="3">
@@ -3535,7 +3665,7 @@
       <c r="E56" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="F56" s="7" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3546,7 +3676,7 @@
       <c r="B57" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="7" t="s">
         <v>126</v>
       </c>
       <c r="D57" s="3">
@@ -3555,7 +3685,7 @@
       <c r="E57" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="F57" s="7" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3566,7 +3696,7 @@
       <c r="B58" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="7" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="3">
@@ -3575,7 +3705,7 @@
       <c r="E58" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="F58" s="7" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3596,10 +3726,10 @@
         <v>1</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="24">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="36">
       <c r="A60" s="3">
         <v>58</v>
       </c>
@@ -3607,7 +3737,7 @@
         <v>134</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>135</v>
+        <v>210</v>
       </c>
       <c r="D60" s="3">
         <v>0</v>
@@ -3616,10 +3746,10 @@
         <v>1</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="24">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="36">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -3627,7 +3757,7 @@
         <v>137</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>138</v>
+        <v>211</v>
       </c>
       <c r="D61" s="3">
         <v>0</v>
@@ -3636,7 +3766,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>139</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -3647,7 +3777,7 @@
         <v>140</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>141</v>
+        <v>222</v>
       </c>
       <c r="D62" s="3">
         <v>0</v>
@@ -3656,10 +3786,10 @@
         <v>1</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="48">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="60">
       <c r="A63" s="3">
         <v>61</v>
       </c>
@@ -3667,7 +3797,7 @@
         <v>8</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>143</v>
+        <v>212</v>
       </c>
       <c r="D63" s="3">
         <v>0</v>
@@ -3676,7 +3806,7 @@
         <v>1</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>144</v>
+        <v>224</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -3687,7 +3817,7 @@
         <v>145</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>146</v>
+        <v>213</v>
       </c>
       <c r="D64" s="3">
         <v>0</v>
@@ -3696,7 +3826,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>147</v>
+        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="48">
@@ -3707,7 +3837,7 @@
         <v>148</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>149</v>
+        <v>214</v>
       </c>
       <c r="D65" s="3">
         <v>0</v>
@@ -3715,8 +3845,8 @@
       <c r="E65" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F65" s="4" t="s">
-        <v>172</v>
+      <c r="F65" s="7" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="24">
@@ -3735,7 +3865,7 @@
       <c r="E66" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F66" s="4" t="s">
+      <c r="F66" s="7" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3747,7 +3877,7 @@
         <v>153</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>154</v>
+        <v>215</v>
       </c>
       <c r="D67" s="3">
         <v>0</v>
@@ -3756,10 +3886,10 @@
         <v>1</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="24">
       <c r="A68" s="3">
         <v>66</v>
       </c>
@@ -3767,7 +3897,7 @@
         <v>156</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>157</v>
+        <v>216</v>
       </c>
       <c r="D68" s="3">
         <v>0</v>
@@ -3776,7 +3906,7 @@
         <v>1</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>158</v>
+        <v>228</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3787,7 +3917,7 @@
         <v>159</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>160</v>
+        <v>217</v>
       </c>
       <c r="D69" s="3">
         <v>0</v>
@@ -3796,10 +3926,10 @@
         <v>1</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="24">
       <c r="A70" s="3">
         <v>72</v>
       </c>
@@ -3807,7 +3937,7 @@
         <v>162</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>163</v>
+        <v>218</v>
       </c>
       <c r="D70" s="3">
         <v>0</v>
@@ -3816,7 +3946,7 @@
         <v>1</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>164</v>
+        <v>230</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="24">
@@ -3827,7 +3957,7 @@
         <v>165</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>166</v>
+        <v>219</v>
       </c>
       <c r="D71" s="3">
         <v>0</v>
@@ -3836,7 +3966,7 @@
         <v>1</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>167</v>
+        <v>231</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="24">
@@ -3846,7 +3976,7 @@
       <c r="B72" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="7" t="s">
         <v>168</v>
       </c>
       <c r="D72" s="3">
@@ -3855,7 +3985,7 @@
       <c r="E72" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F72" s="4" t="s">
+      <c r="F72" s="7" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3866,7 +3996,7 @@
       <c r="B73" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="7" t="s">
         <v>170</v>
       </c>
       <c r="D73" s="3">
@@ -3875,7 +4005,7 @@
       <c r="E73" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F73" s="4" t="s">
+      <c r="F73" s="7" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the code explanations
</commit_message>
<xml_diff>
--- a/code_explanations.xlsx
+++ b/code_explanations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="265">
   <si>
     <t>Kod</t>
   </si>
@@ -713,9 +713,6 @@
     <t>1 if the a folk music piece, 0 else</t>
   </si>
   <si>
-    <t>Soz1=THM (indiced accidentals; b1, b2 etc.), Soz1=TSM (Arel – Ezgi accidentals). Bu takdirde b2’ler b1’e, b3’ler b4’e vb., yani sırasıyla ters ve çengelli bemole vb. dönüştürülmeli), Soz1=Karma (Mus2-Alfadaki yöntem)</t>
-  </si>
-  <si>
     <t>The date of composition written on the Söz1 field</t>
   </si>
   <si>
@@ -779,13 +776,61 @@
     <t>Slides from this note and the next note but does not connect the notes.</t>
   </si>
   <si>
-    <t>Natural Mordan (-)</t>
-  </si>
-  <si>
     <t>Silent natural gracenote (-)</t>
   </si>
   <si>
     <t>The next higher-pitched natural note is played as a silent gracenote.</t>
+  </si>
+  <si>
+    <t>The value is written to the Soz1 field and indicates the accidentals to be used in the prnt. If it is "THM" Turkish folk music accidentals are used (indiced accidentals; b1, b2 etc.), whereas if the value is "TSM" Turkish art music accidentals are printed (Arel – Ezgi accidentals). In case the value is Karma the method in Mus2-Alpha is selected.</t>
+  </si>
+  <si>
+    <t>Phrase Boundary</t>
+  </si>
+  <si>
+    <t>The boundary of a phrase/sentence/motif … Naturally one should assume a boundary at the start and end of the score.</t>
+  </si>
+  <si>
+    <t>Modulation/Flavor Start</t>
+  </si>
+  <si>
+    <t>The modulated note (Söz-1) and makam flavor (Söz-2) are written.</t>
+  </si>
+  <si>
+    <t>Modulation/Flavor End</t>
+  </si>
+  <si>
+    <t>Additional information such as "İnici"/"Çıkıcı" ("Ascending"/"Descending") may be written to the Söz-2 field.</t>
+  </si>
+  <si>
+    <t>Used when switched to a different number of  pulses (zaman) or unit pulset (mertebe) without indicating a usul name.The new values are written to the Pay and Payda fields. It is used to notate the subdivisions of big usuls such as 32/4.</t>
+  </si>
+  <si>
+    <t>Measure change (Rhythm)</t>
+  </si>
+  <si>
+    <t>Makam name is written to Söz1 field and the notes in the key signature  ("B4b1, F5#4",…) are written to Söz2 field</t>
+  </si>
+  <si>
+    <t>Natural Mordent (-)</t>
+  </si>
+  <si>
+    <t>Lower Mordent</t>
+  </si>
+  <si>
+    <t>Natural Lower Mordent (-)</t>
+  </si>
+  <si>
+    <t>Lower Grupetto</t>
+  </si>
+  <si>
+    <t>Natural Grupetto (-)</t>
+  </si>
+  <si>
+    <t>Natural Lower Grupetto (-)</t>
+  </si>
+  <si>
+    <t>Lower Trill</t>
   </si>
 </sst>
 </file>
@@ -910,9 +955,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -956,19 +1003,21 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sayfa1" xfId="1"/>
   </cellStyles>
@@ -2269,7 +2318,7 @@
         <v>115</v>
       </c>
       <c r="G53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="60">
@@ -2290,7 +2339,7 @@
         <v>118</v>
       </c>
       <c r="G54" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="36">
@@ -2686,8 +2735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2806,7 +2855,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2862,7 +2911,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="48">
@@ -3082,14 +3131,14 @@
         <v>54</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="6" t="b">
         <v>1</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="24">
@@ -3100,14 +3149,14 @@
         <v>8</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="6" t="b">
         <v>1</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="24">
@@ -3118,14 +3167,14 @@
         <v>59</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="6" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="24">
@@ -3136,14 +3185,14 @@
         <v>8</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="60">
@@ -3173,8 +3222,8 @@
       <c r="B26" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>68</v>
+      <c r="C26" s="4" t="s">
+        <v>259</v>
       </c>
       <c r="D26" s="3">
         <v>115</v>
@@ -3194,7 +3243,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="6" t="b">
@@ -3211,8 +3260,8 @@
       <c r="B28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>71</v>
+      <c r="C28" s="4" t="s">
+        <v>260</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="6" t="b">
@@ -3237,7 +3286,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G29" s="9"/>
     </row>
@@ -3268,8 +3317,8 @@
       <c r="B31" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>78</v>
+      <c r="C31" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="D31" s="3">
         <v>168</v>
@@ -3288,8 +3337,8 @@
       <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>80</v>
+      <c r="C32" s="4" t="s">
+        <v>262</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="6" t="b">
@@ -3306,8 +3355,8 @@
       <c r="B33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>81</v>
+      <c r="C33" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="6" t="b">
@@ -3324,8 +3373,8 @@
       <c r="B34" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>83</v>
+      <c r="C34" s="4" t="s">
+        <v>264</v>
       </c>
       <c r="D34" s="3">
         <v>165</v>
@@ -3381,7 +3430,7 @@
         <v>87</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D37" s="3">
         <v>212</v>
@@ -3390,7 +3439,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3663,8 +3712,8 @@
       <c r="E52" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F52" s="7" t="s">
-        <v>112</v>
+      <c r="F52" s="4" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="60">
@@ -3700,25 +3749,25 @@
         <v>0</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="36">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="24">
       <c r="A55" s="3">
         <v>53</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C55" s="7" t="s">
-        <v>120</v>
+      <c r="C55" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F55" s="7" t="s">
-        <v>121</v>
+      <c r="F55" s="4" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="24">
@@ -3728,8 +3777,8 @@
       <c r="B56" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="7" t="s">
-        <v>123</v>
+      <c r="C56" s="4" t="s">
+        <v>251</v>
       </c>
       <c r="D56" s="3">
         <v>0</v>
@@ -3737,19 +3786,19 @@
       <c r="E56" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F56" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="F56" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="36">
       <c r="A57" s="3">
         <v>55</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C57" s="7" t="s">
-        <v>126</v>
+      <c r="C57" s="4" t="s">
+        <v>253</v>
       </c>
       <c r="D57" s="3">
         <v>0</v>
@@ -3757,19 +3806,19 @@
       <c r="E57" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F57" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="48">
+      <c r="F57" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="60">
       <c r="A58" s="3">
         <v>56</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C58" s="7" t="s">
-        <v>129</v>
+      <c r="C58" s="4" t="s">
+        <v>256</v>
       </c>
       <c r="D58" s="3">
         <v>0</v>
@@ -3777,8 +3826,8 @@
       <c r="E58" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F58" s="7" t="s">
-        <v>130</v>
+      <c r="F58" s="4" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -3901,7 +3950,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="48">
+    <row r="65" spans="1:6" ht="72">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -3917,8 +3966,8 @@
       <c r="E65" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F65" s="7" t="s">
-        <v>225</v>
+      <c r="F65" s="4" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="24">
@@ -3938,7 +3987,7 @@
         <v>1</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3958,7 +4007,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="24">
@@ -3978,7 +4027,7 @@
         <v>1</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3998,7 +4047,7 @@
         <v>1</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="24">
@@ -4018,7 +4067,7 @@
         <v>1</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="24">
@@ -4038,7 +4087,7 @@
         <v>1</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="24">
@@ -4049,7 +4098,7 @@
         <v>8</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D72" s="3">
         <v>0</v>
@@ -4058,7 +4107,7 @@
         <v>1</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="24">

</xml_diff>